<commit_message>
Adjust number mapping and update xlsx
</commit_message>
<xml_diff>
--- a/mapping.xlsx
+++ b/mapping.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="1">
   <si>
     <t>x</t>
   </si>
@@ -344,10 +344,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AF8" sqref="AF8"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="U34" sqref="U34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -567,37 +567,13 @@
       <c r="J5">
         <v>27</v>
       </c>
-      <c r="M5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N5" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>0</v>
-      </c>
       <c r="P5" t="s">
         <v>0</v>
       </c>
       <c r="R5" t="s">
         <v>0</v>
       </c>
-      <c r="S5" t="s">
-        <v>0</v>
-      </c>
-      <c r="T5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" t="s">
-        <v>0</v>
-      </c>
       <c r="W5" t="s">
-        <v>0</v>
-      </c>
-      <c r="X5" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="s">
         <v>0</v>
       </c>
       <c r="Z5" t="s">
@@ -887,6 +863,513 @@
       </c>
       <c r="K11">
         <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S12" t="s">
+        <v>0</v>
+      </c>
+      <c r="T12" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" t="s">
+        <v>0</v>
+      </c>
+      <c r="W12" t="s">
+        <v>0</v>
+      </c>
+      <c r="X12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R13" t="s">
+        <v>0</v>
+      </c>
+      <c r="S13" t="s">
+        <v>0</v>
+      </c>
+      <c r="T13" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" t="s">
+        <v>0</v>
+      </c>
+      <c r="W13" t="s">
+        <v>0</v>
+      </c>
+      <c r="X13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N15" t="s">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" t="s">
+        <v>0</v>
+      </c>
+      <c r="W15" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="N16" t="s">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>0</v>
+      </c>
+      <c r="R16" t="s">
+        <v>0</v>
+      </c>
+      <c r="S16" t="s">
+        <v>0</v>
+      </c>
+      <c r="T16" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" t="s">
+        <v>0</v>
+      </c>
+      <c r="W16" t="s">
+        <v>0</v>
+      </c>
+      <c r="X16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="N17" t="s">
+        <v>0</v>
+      </c>
+      <c r="O17" t="s">
+        <v>0</v>
+      </c>
+      <c r="R17" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="N18" t="s">
+        <v>0</v>
+      </c>
+      <c r="O18" t="s">
+        <v>0</v>
+      </c>
+      <c r="R18" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
+        <v>0</v>
+      </c>
+      <c r="R19" t="s">
+        <v>0</v>
+      </c>
+      <c r="S19" t="s">
+        <v>0</v>
+      </c>
+      <c r="T19" t="s">
+        <v>0</v>
+      </c>
+      <c r="U19" t="s">
+        <v>0</v>
+      </c>
+      <c r="W19" t="s">
+        <v>0</v>
+      </c>
+      <c r="X19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="N20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>0</v>
+      </c>
+      <c r="R20" t="s">
+        <v>0</v>
+      </c>
+      <c r="S20" t="s">
+        <v>0</v>
+      </c>
+      <c r="T20" t="s">
+        <v>0</v>
+      </c>
+      <c r="U20" t="s">
+        <v>0</v>
+      </c>
+      <c r="W20" t="s">
+        <v>0</v>
+      </c>
+      <c r="X20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M22" t="s">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>0</v>
+      </c>
+      <c r="R22" t="s">
+        <v>0</v>
+      </c>
+      <c r="S22" t="s">
+        <v>0</v>
+      </c>
+      <c r="T22" t="s">
+        <v>0</v>
+      </c>
+      <c r="U22" t="s">
+        <v>0</v>
+      </c>
+      <c r="W22" t="s">
+        <v>0</v>
+      </c>
+      <c r="X22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M23" t="s">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>0</v>
+      </c>
+      <c r="R23" t="s">
+        <v>0</v>
+      </c>
+      <c r="S23" t="s">
+        <v>0</v>
+      </c>
+      <c r="T23" t="s">
+        <v>0</v>
+      </c>
+      <c r="U23" t="s">
+        <v>0</v>
+      </c>
+      <c r="W23" t="s">
+        <v>0</v>
+      </c>
+      <c r="X23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M24" t="s">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>0</v>
+      </c>
+      <c r="R24" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M25" t="s">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>0</v>
+      </c>
+      <c r="R25" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="M26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N26" t="s">
+        <v>0</v>
+      </c>
+      <c r="O26" t="s">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>0</v>
+      </c>
+      <c r="R26" t="s">
+        <v>0</v>
+      </c>
+      <c r="S26" t="s">
+        <v>0</v>
+      </c>
+      <c r="T26" t="s">
+        <v>0</v>
+      </c>
+      <c r="U26" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="P27" t="s">
+        <v>0</v>
+      </c>
+      <c r="R27" t="s">
+        <v>0</v>
+      </c>
+      <c r="U27" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="P28" t="s">
+        <v>0</v>
+      </c>
+      <c r="R28" t="s">
+        <v>0</v>
+      </c>
+      <c r="U28" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="P29" t="s">
+        <v>0</v>
+      </c>
+      <c r="R29" t="s">
+        <v>0</v>
+      </c>
+      <c r="S29" t="s">
+        <v>0</v>
+      </c>
+      <c r="T29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U29" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="P30" t="s">
+        <v>0</v>
+      </c>
+      <c r="R30" t="s">
+        <v>0</v>
+      </c>
+      <c r="S30" t="s">
+        <v>0</v>
+      </c>
+      <c r="T30" t="s">
+        <v>0</v>
+      </c>
+      <c r="U30" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="13:26" x14ac:dyDescent="0.2">
+      <c r="R32" t="s">
+        <v>0</v>
+      </c>
+      <c r="S32" t="s">
+        <v>0</v>
+      </c>
+      <c r="T32" t="s">
+        <v>0</v>
+      </c>
+      <c r="U32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R33" t="s">
+        <v>0</v>
+      </c>
+      <c r="S33" t="s">
+        <v>0</v>
+      </c>
+      <c r="T33" t="s">
+        <v>0</v>
+      </c>
+      <c r="U33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R34" t="s">
+        <v>0</v>
+      </c>
+      <c r="U34" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R35" t="s">
+        <v>0</v>
+      </c>
+      <c r="U35" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R36" t="s">
+        <v>0</v>
+      </c>
+      <c r="U36" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R37" t="s">
+        <v>0</v>
+      </c>
+      <c r="U37" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R38" t="s">
+        <v>0</v>
+      </c>
+      <c r="U38" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R39" t="s">
+        <v>0</v>
+      </c>
+      <c r="S39" t="s">
+        <v>0</v>
+      </c>
+      <c r="T39" t="s">
+        <v>0</v>
+      </c>
+      <c r="U39" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="18:21" x14ac:dyDescent="0.2">
+      <c r="R40" t="s">
+        <v>0</v>
+      </c>
+      <c r="S40" t="s">
+        <v>0</v>
+      </c>
+      <c r="T40" t="s">
+        <v>0</v>
+      </c>
+      <c r="U40" t="s">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>